<commit_message>
Update Nomenclature des composants.xlsx
</commit_message>
<xml_diff>
--- a/Hardware/Nomenclature des composants.xlsx
+++ b/Hardware/Nomenclature des composants.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c1bfb2c967edd544/Documents/GitHub/2324_Projet3DN_AnalyseurQualiteReseauElectrique/Hardware/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliensaint-leger/Documents/GitHub/2324_Projet3DN_AnalyseurQualiteReseauElectrique/Hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="8_{5CD67A80-1F11-4024-8A49-5958BB557664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FC999BE-8A10-45C1-97FF-2752783EC1E0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D7A9BF-5117-1B46-ABB6-B54B966E7718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{25E8B7A7-E779-47F8-9B21-BDA3522EB2ED}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{25E8B7A7-E779-47F8-9B21-BDA3522EB2ED}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
+    <sheet name="Carte Acquisition" sheetId="1" r:id="rId1"/>
+    <sheet name="Carte Traitement" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="42">
   <si>
     <t>Nomenclature des composants</t>
   </si>
@@ -50,12 +50,6 @@
   </si>
   <si>
     <t>Designation</t>
-  </si>
-  <si>
-    <t>Projet Analyseur de réseau électrique</t>
-  </si>
-  <si>
-    <t>Pin out de la carte</t>
   </si>
   <si>
     <t>Capteur de tension</t>
@@ -246,18 +240,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -295,7 +281,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -401,7 +387,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -543,7 +529,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -553,41 +539,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DAC16DD-76D0-4C23-90D5-767943A1EE18}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.54296875" customWidth="1"/>
-    <col min="3" max="3" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>2</v>
@@ -596,13 +582,13 @@
         <v>3</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -610,15 +596,15 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1">
         <v>1617416</v>
@@ -630,14 +616,14 @@
         <v>77.53</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I7">
         <f>E7*F7</f>
         <v>232.59</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="1"/>
@@ -649,15 +635,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1">
         <v>3224813</v>
@@ -669,22 +655,22 @@
         <v>5.81</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
         <v>5.81</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D10" s="1">
         <v>3224811</v>
@@ -696,22 +682,22 @@
         <v>5.65</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
         <v>5.65</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D11" s="1">
         <v>3224810</v>
@@ -723,22 +709,22 @@
         <v>5.43</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
         <v>5.43</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D12" s="1">
         <v>3224814</v>
@@ -750,14 +736,14 @@
         <v>5.76</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
         <v>5.76</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -769,18 +755,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E14" s="2">
         <v>1</v>
@@ -789,14 +775,14 @@
         <v>40.39</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I14">
         <f t="shared" si="0"/>
         <v>40.39</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -808,18 +794,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E16" s="2">
         <v>1</v>
@@ -828,14 +814,14 @@
         <v>3.58</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I16">
         <f t="shared" si="0"/>
         <v>3.58</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -847,15 +833,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="D18" s="1">
         <v>3122059</v>
@@ -867,13 +853,13 @@
         <v>0</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I18">
         <v>2.41</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -885,15 +871,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="D20" s="1">
         <v>4021486</v>
@@ -905,7 +891,7 @@
         <v>4.13</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2">
@@ -913,7 +899,7 @@
         <v>28.91</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -921,9 +907,9 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -934,7 +920,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -942,7 +928,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -950,7 +936,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -958,7 +944,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -966,7 +952,7 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -974,7 +960,7 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -982,7 +968,7 @@
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -990,7 +976,7 @@
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -998,7 +984,7 @@
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -1006,7 +992,7 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -1014,7 +1000,7 @@
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -1022,7 +1008,7 @@
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -1040,30 +1026,120 @@
     <hyperlink ref="C20" r:id="rId6" tooltip="OP275GSZ" display="https://fr.farnell.com/analog-devices/op275gsz/ampli-op-9mhz-40-a-85-c-nsoic/dp/4021486?st=op275" xr:uid="{8E5C894A-2517-47D1-997C-6B89569E0635}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K008000 Interne SNCF Réseau</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66EA6A3A-C436-48FD-B3AE-2362EEAC2785}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.5" customWidth="1"/>
+    <col min="4" max="4" width="25.1640625" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" customWidth="1"/>
+    <col min="9" max="9" width="13.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>6</v>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K008000 Interne SNCF Réseau</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>